<commit_message>
Create model class (gun, company).
</commit_message>
<xml_diff>
--- a/team03.xlsx
+++ b/team03.xlsx
@@ -967,7 +967,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2449,7 +2449,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>